<commit_message>
1.0.9003 Added new DSMZ numbers
</commit_message>
<xml_diff>
--- a/inst/app/resources/ElenMatchR_template.xlsx
+++ b/inst/app/resources/ElenMatchR_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/turnbaughlab/qb3share/jbisanz/ElGenomes2019/ElenMatchR_v1.0/ElenMatchR/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/turnbaughlab/qb3share/jbisanz/ElGenomes2019/ElenMatchR_v1.0/ElenMatchR/inst/app/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489A7C06-C376-3B43-B68B-CF537ED9F39E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B2E039-7148-8D48-AB75-B396FFD57B96}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35660" windowHeight="23220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Genomes" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="401">
   <si>
     <t>Adlercreutzia_equolifaciens_DSM19450</t>
   </si>
@@ -297,9 +297,6 @@
     <t>Eggerthella lenta C592</t>
   </si>
   <si>
-    <t>Eggerthella lenta DIAB165</t>
-  </si>
-  <si>
     <t>Eggerthella lenta DIAB223</t>
   </si>
   <si>
@@ -544,12 +541,6 @@
   </si>
   <si>
     <t>El CC8/6 D5 4</t>
-  </si>
-  <si>
-    <t>El DIAB165</t>
-  </si>
-  <si>
-    <t>El DIAB223</t>
   </si>
   <si>
     <t>El DSM 11767</t>
@@ -1180,13 +1171,91 @@
     <t>Your_Phenotype</t>
   </si>
   <si>
-    <t>#To add custom phenotypes, change Your_Phenotype to the desired description  and fill in names of categorical variables below. Strain_Name and GenomeID columns must not be changed.</t>
-  </si>
-  <si>
     <t>Strain_Name</t>
   </si>
   <si>
     <t>PTJ0094</t>
+  </si>
+  <si>
+    <t>DSM110904</t>
+  </si>
+  <si>
+    <t>DSM110905</t>
+  </si>
+  <si>
+    <t>DSM110906</t>
+  </si>
+  <si>
+    <t>DSM110907</t>
+  </si>
+  <si>
+    <t>DSM110908</t>
+  </si>
+  <si>
+    <t>DSM110909</t>
+  </si>
+  <si>
+    <t>DSM110910</t>
+  </si>
+  <si>
+    <t>DSM110911</t>
+  </si>
+  <si>
+    <t>DSM110912</t>
+  </si>
+  <si>
+    <t>DSM110913</t>
+  </si>
+  <si>
+    <t>DSM110914</t>
+  </si>
+  <si>
+    <t>DSM110915</t>
+  </si>
+  <si>
+    <t>DSM110916</t>
+  </si>
+  <si>
+    <t>DSM110917</t>
+  </si>
+  <si>
+    <t>DSM110918</t>
+  </si>
+  <si>
+    <t>Eggerthella lenta RJX1626</t>
+  </si>
+  <si>
+    <t>El RJX1626</t>
+  </si>
+  <si>
+    <t>El RJX1627</t>
+  </si>
+  <si>
+    <t>DSM110919</t>
+  </si>
+  <si>
+    <t>DSM110920</t>
+  </si>
+  <si>
+    <t>DSM110921</t>
+  </si>
+  <si>
+    <t>DSM110922</t>
+  </si>
+  <si>
+    <t>DSM110923</t>
+  </si>
+  <si>
+    <t>DSM110924</t>
+  </si>
+  <si>
+    <t>DSM110925</t>
+  </si>
+  <si>
+    <t>DSM110927</t>
+  </si>
+  <si>
+    <t># Template v1.0.9003: To add custom phenotypes, change Your_Phenotype to the desired description  and fill in names of categorical variables below. Strain_Name and GenomeID columns must not be changed.</t>
   </si>
 </sst>
 </file>
@@ -2091,16 +2160,16 @@
   <dimension ref="A1:F97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="37.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="58.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
@@ -2108,16 +2177,16 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>375</v>
+        <v>400</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1">
       <c r="A2" s="8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>76</v>
@@ -2129,34 +2198,34 @@
         <v>75</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1">
       <c r="A3" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="5" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>0</v>
@@ -2164,44 +2233,44 @@
     </row>
     <row r="5" spans="1:6" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="5" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="5" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>1</v>
@@ -2212,10 +2281,10 @@
         <v>78</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>2</v>
@@ -2223,28 +2292,28 @@
     </row>
     <row r="9" spans="1:6" s="5" customFormat="1">
       <c r="A9" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>3</v>
@@ -2252,16 +2321,16 @@
     </row>
     <row r="11" spans="1:6" s="5" customFormat="1">
       <c r="A11" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>4</v>
@@ -2269,43 +2338,43 @@
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1">
       <c r="A12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="5" customFormat="1">
       <c r="A13" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="5" customFormat="1">
       <c r="A14" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>5</v>
@@ -2313,14 +2382,14 @@
     </row>
     <row r="15" spans="1:6" s="5" customFormat="1">
       <c r="A15" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>6</v>
@@ -2328,13 +2397,13 @@
     </row>
     <row r="16" spans="1:6" s="5" customFormat="1" ht="19">
       <c r="A16" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>7</v>
@@ -2342,13 +2411,16 @@
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="19">
       <c r="A17" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>374</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>8</v>
@@ -2358,11 +2430,14 @@
       <c r="A18" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="B18" s="5" t="s">
+        <v>375</v>
+      </c>
       <c r="C18" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>9</v>
@@ -2370,13 +2445,16 @@
     </row>
     <row r="19" spans="1:5" s="5" customFormat="1">
       <c r="A19" s="5" t="s">
-        <v>243</v>
+        <v>240</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>376</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>10</v>
@@ -2386,11 +2464,14 @@
       <c r="A20" s="5" t="s">
         <v>80</v>
       </c>
+      <c r="B20" s="5" t="s">
+        <v>377</v>
+      </c>
       <c r="C20" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>11</v>
@@ -2401,10 +2482,10 @@
         <v>81</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>12</v>
@@ -2416,7 +2497,7 @@
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>13</v>
@@ -2426,11 +2507,14 @@
       <c r="A23" s="5" t="s">
         <v>83</v>
       </c>
+      <c r="B23" s="5" t="s">
+        <v>378</v>
+      </c>
       <c r="C23" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>14</v>
@@ -2440,11 +2524,14 @@
       <c r="A24" s="5" t="s">
         <v>84</v>
       </c>
+      <c r="B24" s="5" t="s">
+        <v>379</v>
+      </c>
       <c r="C24" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>15</v>
@@ -2452,13 +2539,16 @@
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1">
       <c r="A25" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>380</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>16</v>
@@ -2468,11 +2558,14 @@
       <c r="A26" s="5" t="s">
         <v>85</v>
       </c>
+      <c r="B26" s="5" t="s">
+        <v>381</v>
+      </c>
       <c r="C26" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>17</v>
@@ -2480,13 +2573,16 @@
     </row>
     <row r="27" spans="1:5" s="5" customFormat="1">
       <c r="A27" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>382</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>18</v>
@@ -2494,13 +2590,16 @@
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1">
       <c r="A28" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>383</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>19</v>
@@ -2510,11 +2609,14 @@
       <c r="A29" s="5" t="s">
         <v>86</v>
       </c>
+      <c r="B29" s="5" t="s">
+        <v>384</v>
+      </c>
       <c r="C29" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>20</v>
@@ -2522,16 +2624,16 @@
     </row>
     <row r="30" spans="1:5" s="5" customFormat="1">
       <c r="A30" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>21</v>
@@ -2543,7 +2645,7 @@
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>22</v>
@@ -2551,13 +2653,16 @@
     </row>
     <row r="32" spans="1:5" s="5" customFormat="1">
       <c r="A32" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>23</v>
@@ -2565,13 +2670,16 @@
     </row>
     <row r="33" spans="1:5" s="5" customFormat="1">
       <c r="A33" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>386</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>24</v>
@@ -2579,13 +2687,16 @@
     </row>
     <row r="34" spans="1:5" s="5" customFormat="1">
       <c r="A34" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>387</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>25</v>
@@ -2593,13 +2704,16 @@
     </row>
     <row r="35" spans="1:5" s="5" customFormat="1">
       <c r="A35" s="5" t="s">
-        <v>88</v>
+        <v>389</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>388</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>171</v>
+        <v>390</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>26</v>
@@ -2607,13 +2721,13 @@
     </row>
     <row r="36" spans="1:5" s="5" customFormat="1">
       <c r="A36" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>172</v>
+        <v>391</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>27</v>
@@ -2621,16 +2735,16 @@
     </row>
     <row r="37" spans="1:5" s="5" customFormat="1">
       <c r="A37" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>28</v>
@@ -2638,16 +2752,16 @@
     </row>
     <row r="38" spans="1:5" s="5" customFormat="1">
       <c r="A38" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>29</v>
@@ -2655,16 +2769,16 @@
     </row>
     <row r="39" spans="1:5" s="5" customFormat="1">
       <c r="A39" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>30</v>
@@ -2672,16 +2786,16 @@
     </row>
     <row r="40" spans="1:5" s="5" customFormat="1">
       <c r="A40" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>31</v>
@@ -2689,28 +2803,31 @@
     </row>
     <row r="41" spans="1:5" s="5" customFormat="1">
       <c r="A41" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="5" customFormat="1">
       <c r="A42" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>392</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>32</v>
@@ -2718,13 +2835,16 @@
     </row>
     <row r="43" spans="1:5" s="5" customFormat="1">
       <c r="A43" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>393</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>33</v>
@@ -2732,11 +2852,11 @@
     </row>
     <row r="44" spans="1:5" s="5" customFormat="1">
       <c r="A44" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>34</v>
@@ -2744,11 +2864,11 @@
     </row>
     <row r="45" spans="1:5" s="5" customFormat="1">
       <c r="A45" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>35</v>
@@ -2756,11 +2876,11 @@
     </row>
     <row r="46" spans="1:5" s="5" customFormat="1">
       <c r="A46" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>36</v>
@@ -2768,11 +2888,11 @@
     </row>
     <row r="47" spans="1:5" s="5" customFormat="1">
       <c r="A47" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>37</v>
@@ -2780,11 +2900,11 @@
     </row>
     <row r="48" spans="1:5" s="5" customFormat="1">
       <c r="A48" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>38</v>
@@ -2792,11 +2912,11 @@
     </row>
     <row r="49" spans="1:5" s="5" customFormat="1">
       <c r="A49" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>39</v>
@@ -2804,11 +2924,11 @@
     </row>
     <row r="50" spans="1:5" s="5" customFormat="1">
       <c r="A50" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>40</v>
@@ -2816,11 +2936,11 @@
     </row>
     <row r="51" spans="1:5" s="5" customFormat="1">
       <c r="A51" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>41</v>
@@ -2828,11 +2948,11 @@
     </row>
     <row r="52" spans="1:5" s="5" customFormat="1">
       <c r="A52" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>42</v>
@@ -2840,11 +2960,11 @@
     </row>
     <row r="53" spans="1:5" s="5" customFormat="1">
       <c r="A53" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>43</v>
@@ -2852,11 +2972,11 @@
     </row>
     <row r="54" spans="1:5" s="5" customFormat="1">
       <c r="A54" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>44</v>
@@ -2864,11 +2984,11 @@
     </row>
     <row r="55" spans="1:5" s="5" customFormat="1">
       <c r="A55" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>45</v>
@@ -2876,11 +2996,11 @@
     </row>
     <row r="56" spans="1:5" s="5" customFormat="1">
       <c r="A56" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>46</v>
@@ -2888,13 +3008,16 @@
     </row>
     <row r="57" spans="1:5" s="5" customFormat="1">
       <c r="A57" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>394</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>47</v>
@@ -2902,13 +3025,16 @@
     </row>
     <row r="58" spans="1:5" s="5" customFormat="1">
       <c r="A58" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>395</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>48</v>
@@ -2916,13 +3042,13 @@
     </row>
     <row r="59" spans="1:5" s="5" customFormat="1">
       <c r="A59" s="5" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>49</v>
@@ -2930,11 +3056,11 @@
     </row>
     <row r="60" spans="1:5" s="5" customFormat="1">
       <c r="A60" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>50</v>
@@ -2942,16 +3068,16 @@
     </row>
     <row r="61" spans="1:5" s="5" customFormat="1">
       <c r="A61" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>51</v>
@@ -2959,13 +3085,13 @@
     </row>
     <row r="62" spans="1:5" s="5" customFormat="1">
       <c r="A62" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>52</v>
@@ -2973,13 +3099,16 @@
     </row>
     <row r="63" spans="1:5" s="5" customFormat="1">
       <c r="A63" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>396</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>53</v>
@@ -2987,16 +3116,16 @@
     </row>
     <row r="64" spans="1:5" s="5" customFormat="1">
       <c r="A64" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>54</v>
@@ -3004,11 +3133,11 @@
     </row>
     <row r="65" spans="1:5" s="5" customFormat="1">
       <c r="A65" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>55</v>
@@ -3016,11 +3145,11 @@
     </row>
     <row r="66" spans="1:5" s="5" customFormat="1">
       <c r="A66" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>56</v>
@@ -3028,44 +3157,44 @@
     </row>
     <row r="67" spans="1:5" s="5" customFormat="1">
       <c r="A67" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="5" customFormat="1">
       <c r="A68" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="5" customFormat="1">
       <c r="A69" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>57</v>
@@ -3073,14 +3202,14 @@
     </row>
     <row r="70" spans="1:5" s="5" customFormat="1">
       <c r="A70" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>58</v>
@@ -3088,13 +3217,16 @@
     </row>
     <row r="71" spans="1:5" s="5" customFormat="1">
       <c r="A71" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>397</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>59</v>
@@ -3102,30 +3234,33 @@
     </row>
     <row r="72" spans="1:5" s="5" customFormat="1">
       <c r="A72" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="5" customFormat="1">
       <c r="A73" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>398</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>60</v>
@@ -3133,46 +3268,46 @@
     </row>
     <row r="74" spans="1:5" s="5" customFormat="1">
       <c r="A74" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="5" customFormat="1">
       <c r="A75" s="5" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="5" customFormat="1">
       <c r="A76" s="5" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>61</v>
@@ -3180,29 +3315,29 @@
     </row>
     <row r="77" spans="1:5" s="5" customFormat="1">
       <c r="A77" s="5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="5" customFormat="1">
       <c r="A78" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>62</v>
@@ -3210,43 +3345,45 @@
     </row>
     <row r="79" spans="1:5" s="5" customFormat="1">
       <c r="A79" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E79" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="5" customFormat="1">
       <c r="A80" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="5" customFormat="1">
       <c r="A81" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B81" s="10"/>
+        <v>138</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>399</v>
+      </c>
       <c r="C81" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>63</v>
@@ -3254,29 +3391,29 @@
     </row>
     <row r="82" spans="1:5" s="5" customFormat="1">
       <c r="A82" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="5" customFormat="1">
       <c r="A83" s="5" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>64</v>
@@ -3284,14 +3421,14 @@
     </row>
     <row r="84" spans="1:5" s="5" customFormat="1">
       <c r="A84" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C84" s="7"/>
       <c r="D84" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>65</v>
@@ -3299,14 +3436,14 @@
     </row>
     <row r="85" spans="1:5" s="5" customFormat="1">
       <c r="A85" s="5" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>66</v>
@@ -3314,28 +3451,28 @@
     </row>
     <row r="86" spans="1:5" s="5" customFormat="1">
       <c r="A86" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="5" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="5" customFormat="1">
       <c r="A87" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>67</v>
@@ -3343,14 +3480,14 @@
     </row>
     <row r="88" spans="1:5" s="5" customFormat="1">
       <c r="A88" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>68</v>
@@ -3358,14 +3495,14 @@
     </row>
     <row r="89" spans="1:5" s="5" customFormat="1">
       <c r="A89" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>69</v>
@@ -3373,48 +3510,48 @@
     </row>
     <row r="90" spans="1:5" s="5" customFormat="1">
       <c r="A90" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="5" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="5" customFormat="1">
       <c r="A91" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="4" customFormat="1">
       <c r="A92" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>70</v>
@@ -3422,16 +3559,16 @@
     </row>
     <row r="93" spans="1:5" s="4" customFormat="1">
       <c r="A93" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>71</v>
@@ -3439,14 +3576,14 @@
     </row>
     <row r="94" spans="1:5" s="4" customFormat="1">
       <c r="A94" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>72</v>
@@ -3454,16 +3591,16 @@
     </row>
     <row r="95" spans="1:5" s="4" customFormat="1">
       <c r="A95" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>73</v>
@@ -3471,13 +3608,13 @@
     </row>
     <row r="96" spans="1:5" s="4" customFormat="1">
       <c r="A96" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>74</v>
@@ -3485,17 +3622,17 @@
     </row>
     <row r="97" spans="1:5" s="4" customFormat="1">
       <c r="A97" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C97" s="6"/>
       <c r="D97" s="4" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>